<commit_message>
Add Multilabel (Native) for AutoGluon
</commit_message>
<xml_diff>
--- a/results/binary/1462/automl.xlsx
+++ b/results/binary/1462/automl.xlsx
@@ -473,17 +473,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>00:00:44 (00:02:51 Â± 00:01:34)</t>
+          <t>00:00:44 (00:02:51 ± 00:01:34)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00:00:05 (00:00:06 Â± 00:00:00)</t>
+          <t>00:00:05 (00:00:06 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,17 +503,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.000 (0.995 Â± 0.005)</t>
+          <t>1.000 (0.995 ± 0.005)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>00:00:07 (00:00:11 Â± 00:00:03)</t>
+          <t>00:00:07 (00:00:11 ± 00:00:03)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,17 +535,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>00:00:30 (00:00:38 Â± 00:00:06)</t>
+          <t>00:00:30 (00:00:38 ± 00:00:06)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -567,17 +567,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.000 (0.999 Â± 0.003)</t>
+          <t>1.000 (0.999 ± 0.003)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>00:05:06 (00:05:12 Â± 00:00:03)</t>
+          <t>00:05:06 (00:05:12 ± 00:00:03)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:00:01 (00:00:02 Â± 00:00:00)</t>
+          <t>00:00:01 (00:00:02 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -599,17 +599,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.001)</t>
+          <t>1.000 (1.000 ± 0.001)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>00:04:57 (00:05:01 Â± 00:00:02)</t>
+          <t>00:04:57 (00:05:01 ± 00:00:02)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -631,17 +631,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.956 (0.932 Â± 0.013)</t>
+          <t>0.956 (0.932 ± 0.013)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>00:05:00 (00:05:04 Â± 00:00:02)</t>
+          <t>00:05:00 (00:05:04 ± 00:00:02)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -663,17 +663,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.000 (0.993 Â± 0.010)</t>
+          <t>1.000 (0.993 ± 0.010)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>00:02:47 (00:04:19 Â± 00:01:02)</t>
+          <t>00:02:47 (00:04:19 ± 00:01:02)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -695,17 +695,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1.000 (0.997 Â± 0.004)</t>
+          <t>1.000 (0.997 ± 0.004)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>00:04:59 (00:05:00 Â± 00:00:00)</t>
+          <t>00:04:59 (00:05:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -727,17 +727,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.000 (0.999 Â± 0.002)</t>
+          <t>1.000 (0.999 ± 0.002)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>00:04:29 (00:04:29 Â± 00:00:00)</t>
+          <t>00:04:29 (00:04:29 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -759,17 +759,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.890 (0.701 Â± 0.154)</t>
+          <t>0.890 (0.701 ± 0.154)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>00:05:01 (00:05:05 Â± 00:00:00)</t>
+          <t>00:05:01 (00:05:05 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -791,17 +791,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.463 (0.399 Â± 0.030)</t>
+          <t>0.463 (0.399 ± 0.030)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>00:02:53 (00:03:13 Â± 00:00:07)</t>
+          <t>00:02:53 (00:03:13 ± 00:00:07)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -823,17 +823,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1.000 (0.997 Â± 0.005)</t>
+          <t>1.000 (0.997 ± 0.005)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>00:00:02 (00:00:14 Â± 00:00:07)</t>
+          <t>00:00:02 (00:00:14 ± 00:00:07)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -855,17 +855,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1.000 (0.994 Â± 0.006)</t>
+          <t>1.000 (0.994 ± 0.006)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>00:00:20 (00:00:23 Â± 00:00:02)</t>
+          <t>00:00:20 (00:00:23 ± 00:00:02)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -887,17 +887,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:10 Â± 00:00:06)</t>
+          <t>00:00:00 (00:00:10 ± 00:00:06)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -919,17 +919,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.001)</t>
+          <t>1.000 (1.000 ± 0.001)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>00:00:08 (00:00:09 Â± 00:00:00)</t>
+          <t>00:00:08 (00:00:09 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -951,17 +951,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>00:05:01 (00:05:18 Â± 00:00:13)</t>
+          <t>00:05:01 (00:05:18 ± 00:00:13)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">

</xml_diff>

<commit_message>
Fixes, updates, and results for 2025
</commit_message>
<xml_diff>
--- a/results/binary/1462/automl.xlsx
+++ b/results/binary/1462/automl.xlsx
@@ -473,17 +473,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>00:00:44 (00:02:51 Â± 00:01:34)</t>
+          <t>00:00:44 (00:02:51 ± 00:01:34)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00:00:05 (00:00:06 Â± 00:00:00)</t>
+          <t>00:00:05 (00:00:06 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,17 +503,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.000 (0.995 Â± 0.005)</t>
+          <t>1.000 (0.995 ± 0.005)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>00:00:07 (00:00:11 Â± 00:00:03)</t>
+          <t>00:00:07 (00:00:11 ± 00:00:03)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,17 +535,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>00:00:30 (00:00:38 Â± 00:00:06)</t>
+          <t>00:00:30 (00:00:38 ± 00:00:06)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -567,17 +567,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.000 (0.999 Â± 0.003)</t>
+          <t>1.000 (0.999 ± 0.003)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>00:05:06 (00:05:12 Â± 00:00:03)</t>
+          <t>00:05:06 (00:05:12 ± 00:00:03)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:00:01 (00:00:02 Â± 00:00:00)</t>
+          <t>00:00:01 (00:00:02 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -599,17 +599,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.001)</t>
+          <t>1.000 (1.000 ± 0.001)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>00:04:57 (00:05:01 Â± 00:00:02)</t>
+          <t>00:04:57 (00:05:01 ± 00:00:02)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -631,17 +631,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.956 (0.932 Â± 0.013)</t>
+          <t>0.956 (0.932 ± 0.013)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>00:05:00 (00:05:04 Â± 00:00:02)</t>
+          <t>00:05:00 (00:05:04 ± 00:00:02)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -663,17 +663,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.000 (0.993 Â± 0.010)</t>
+          <t>1.000 (0.993 ± 0.010)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>00:02:47 (00:04:19 Â± 00:01:02)</t>
+          <t>00:02:47 (00:04:19 ± 00:01:02)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -695,17 +695,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1.000 (0.997 Â± 0.004)</t>
+          <t>1.000 (0.997 ± 0.004)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>00:04:59 (00:05:00 Â± 00:00:00)</t>
+          <t>00:04:59 (00:05:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -727,17 +727,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.000 (0.999 Â± 0.002)</t>
+          <t>1.000 (0.999 ± 0.002)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>00:04:29 (00:04:29 Â± 00:00:00)</t>
+          <t>00:04:29 (00:04:29 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -759,17 +759,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.890 (0.701 Â± 0.154)</t>
+          <t>0.890 (0.701 ± 0.154)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>00:05:01 (00:05:05 Â± 00:00:00)</t>
+          <t>00:05:01 (00:05:05 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -791,17 +791,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.463 (0.399 Â± 0.030)</t>
+          <t>0.463 (0.399 ± 0.030)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>00:02:53 (00:03:13 Â± 00:00:07)</t>
+          <t>00:02:53 (00:03:13 ± 00:00:07)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -823,17 +823,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1.000 (0.997 Â± 0.005)</t>
+          <t>1.000 (0.997 ± 0.005)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>00:00:02 (00:00:14 Â± 00:00:07)</t>
+          <t>00:00:02 (00:00:14 ± 00:00:07)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -855,17 +855,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1.000 (0.994 Â± 0.006)</t>
+          <t>1.000 (0.994 ± 0.006)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>00:00:20 (00:00:23 Â± 00:00:02)</t>
+          <t>00:00:20 (00:00:23 ± 00:00:02)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -887,17 +887,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:10 Â± 00:00:06)</t>
+          <t>00:00:00 (00:00:10 ± 00:00:06)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -919,17 +919,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.001)</t>
+          <t>1.000 (1.000 ± 0.001)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>00:00:08 (00:00:09 Â± 00:00:00)</t>
+          <t>00:00:08 (00:00:09 ± 00:00:00)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -951,17 +951,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1.000 (1.000 Â± 0.000)</t>
+          <t>1.000 (1.000 ± 0.000)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>00:05:01 (00:05:18 Â± 00:00:13)</t>
+          <t>00:05:01 (00:05:18 ± 00:00:13)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+          <t>00:00:00 (00:00:00 ± 00:00:00)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">

</xml_diff>